<commit_message>
Added new Titan Clone link - much better quality
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="325" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{FC616191-BDC2-4A19-95EA-3BDF8126B4A4}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{257ABE13-9F56-48B8-AFCC-7F4097E34692}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -20,6 +20,13 @@
     <sheet name="Bundle Order List" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1076,9 +1083,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2077,9 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2536,23 +2541,23 @@
     <hyperlink ref="B11" r:id="rId5" xr:uid="{0BA4E21B-2D6F-419E-BB1C-022ED717A36F}"/>
     <hyperlink ref="B14" r:id="rId6" xr:uid="{94C4C13B-0BBB-4F7B-A730-B3205BF6E8ED}"/>
     <hyperlink ref="B23" r:id="rId7" xr:uid="{36DCFF59-08CA-412B-82D6-7AAD9283F4CA}"/>
-    <hyperlink ref="B20" r:id="rId8" display="J-Head/E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
-    <hyperlink ref="B21" r:id="rId9" xr:uid="{BB4FD47C-E877-4261-A969-740DE1E39AB4}"/>
-    <hyperlink ref="B27" r:id="rId10" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
-    <hyperlink ref="B17" r:id="rId11" xr:uid="{13ECE8A0-6EE8-4028-9765-E96A93DC6FCD}"/>
-    <hyperlink ref="B9" r:id="rId12" xr:uid="{2A7E1508-6E65-4E26-BF99-CF81B8D345E1}"/>
-    <hyperlink ref="B26" r:id="rId13" xr:uid="{25020B41-41DF-478E-89B1-FE4B385546EA}"/>
-    <hyperlink ref="B19" r:id="rId14" xr:uid="{94831F77-CC8B-4258-8675-6442526C91B3}"/>
-    <hyperlink ref="B12" r:id="rId15" xr:uid="{007564D3-D88A-459E-82C7-E7C8214C723F}"/>
-    <hyperlink ref="B13" r:id="rId16" xr:uid="{4B39742A-81FB-4551-BEF4-69D5B4E51D2B}"/>
-    <hyperlink ref="B15" r:id="rId17" xr:uid="{37CE46E6-337E-4932-891F-7ABBCC15C26A}"/>
-    <hyperlink ref="B22" r:id="rId18" display="BL Touch Probe" xr:uid="{4921FFD9-8616-4796-AF0F-67C77EA5A27C}"/>
-    <hyperlink ref="C22" r:id="rId19" xr:uid="{D8FBE80D-6647-42BD-AA31-6FB3B8A2D48A}"/>
-    <hyperlink ref="C21" r:id="rId20" xr:uid="{55B76075-89E5-4B66-9E0E-72A33EE17BD5}"/>
-    <hyperlink ref="B28" r:id="rId21" xr:uid="{20CA74F6-9B49-4A6D-8DB6-16AFDE7D4641}"/>
-    <hyperlink ref="B24" r:id="rId22" xr:uid="{B94573F1-B78C-47F1-B3ED-C228D2514D12}"/>
-    <hyperlink ref="B25" r:id="rId23" xr:uid="{42695F20-A1CA-4BFF-B93A-3229A8617449}"/>
-    <hyperlink ref="C20" r:id="rId24" display="e3d Type Hotend" xr:uid="{E84D0B7A-20D8-46FC-A33D-C20E4015FB33}"/>
+    <hyperlink ref="B21" r:id="rId8" xr:uid="{BB4FD47C-E877-4261-A969-740DE1E39AB4}"/>
+    <hyperlink ref="B27" r:id="rId9" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
+    <hyperlink ref="B17" r:id="rId10" xr:uid="{13ECE8A0-6EE8-4028-9765-E96A93DC6FCD}"/>
+    <hyperlink ref="B9" r:id="rId11" xr:uid="{2A7E1508-6E65-4E26-BF99-CF81B8D345E1}"/>
+    <hyperlink ref="B26" r:id="rId12" xr:uid="{25020B41-41DF-478E-89B1-FE4B385546EA}"/>
+    <hyperlink ref="B19" r:id="rId13" xr:uid="{94831F77-CC8B-4258-8675-6442526C91B3}"/>
+    <hyperlink ref="B12" r:id="rId14" xr:uid="{007564D3-D88A-459E-82C7-E7C8214C723F}"/>
+    <hyperlink ref="B13" r:id="rId15" xr:uid="{4B39742A-81FB-4551-BEF4-69D5B4E51D2B}"/>
+    <hyperlink ref="B15" r:id="rId16" xr:uid="{37CE46E6-337E-4932-891F-7ABBCC15C26A}"/>
+    <hyperlink ref="B22" r:id="rId17" display="BL Touch Probe" xr:uid="{4921FFD9-8616-4796-AF0F-67C77EA5A27C}"/>
+    <hyperlink ref="C22" r:id="rId18" xr:uid="{D8FBE80D-6647-42BD-AA31-6FB3B8A2D48A}"/>
+    <hyperlink ref="C21" r:id="rId19" xr:uid="{55B76075-89E5-4B66-9E0E-72A33EE17BD5}"/>
+    <hyperlink ref="B28" r:id="rId20" xr:uid="{20CA74F6-9B49-4A6D-8DB6-16AFDE7D4641}"/>
+    <hyperlink ref="B24" r:id="rId21" xr:uid="{B94573F1-B78C-47F1-B3ED-C228D2514D12}"/>
+    <hyperlink ref="B25" r:id="rId22" xr:uid="{42695F20-A1CA-4BFF-B93A-3229A8617449}"/>
+    <hyperlink ref="C20" r:id="rId23" display="e3d Type Hotend" xr:uid="{E84D0B7A-20D8-46FC-A33D-C20E4015FB33}"/>
+    <hyperlink ref="B20" r:id="rId24" display="J-Head/E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>

</xml_diff>

<commit_message>
changing name on upgrade folder to optional stl
also adding x carrier clean
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{257ABE13-9F56-48B8-AFCC-7F4097E34692}"/>
+  <xr:revisionPtr revIDLastSave="336" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{257ABE13-9F56-48B8-AFCC-7F4097E34692}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -1770,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -2084,7 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
updated bowden support bracket
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="336" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{257ABE13-9F56-48B8-AFCC-7F4097E34692}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A4853933-9075-4FD1-8E42-3FACC9A9FEE0}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -266,9 +266,6 @@
     <t>LCD Controller Panel</t>
   </si>
   <si>
-    <t>Layer Fan</t>
-  </si>
-  <si>
     <t>Fan for filament cooling</t>
   </si>
   <si>
@@ -377,9 +374,6 @@
     <t>Filament Extruder</t>
   </si>
   <si>
-    <t>Add Price</t>
-  </si>
-  <si>
     <t>Bulk Price</t>
   </si>
   <si>
@@ -474,6 +468,12 @@
   </si>
   <si>
     <t>5mm X 555 mm Steel rod</t>
+  </si>
+  <si>
+    <t>12V Layer Fan</t>
+  </si>
+  <si>
+    <t>Clone Price</t>
   </si>
 </sst>
 </file>
@@ -1770,7 +1770,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{252991A0-F9B1-4FB6-901D-4CCB3A2906EB}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -1782,7 +1782,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B1" s="37"/>
       <c r="C1" s="37"/>
@@ -1796,7 +1796,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1810,7 +1810,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B6" s="27">
         <f>'V-Slots and Wheels List'!F17</f>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B7" s="27">
         <f>'Component Part List'!E29</f>
@@ -1856,7 +1856,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="27">
         <f>'Fasteners List'!E33</f>
@@ -1869,7 +1869,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
@@ -1878,12 +1878,12 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A13" s="25" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1921,10 +1921,10 @@
   <sheetData>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="33" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1939,10 +1939,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2031,7 +2031,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D15" s="3">
         <v>21</v>
@@ -2053,7 +2053,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
@@ -2062,12 +2062,12 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A20" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2084,7 +2084,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2098,12 +2100,12 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2117,10 +2119,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -2149,7 +2151,7 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2166,7 +2168,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2177,10 +2179,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
@@ -2195,10 +2197,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
         <v>65</v>
@@ -2212,13 +2214,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -2229,13 +2231,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s">
         <v>93</v>
-      </c>
-      <c r="C13" t="s">
-        <v>94</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2266,10 +2268,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -2284,10 +2286,10 @@
         <v>61</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2301,10 +2303,10 @@
         <v>61</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
         <v>80</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2353,10 +2355,10 @@
         <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2365,7 +2367,7 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2373,10 +2375,10 @@
         <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2385,7 +2387,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2393,10 +2395,10 @@
         <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2405,7 +2407,7 @@
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2413,7 +2415,7 @@
         <v>69</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -2467,7 +2469,7 @@
         <v>28</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -2481,10 +2483,10 @@
         <v>61</v>
       </c>
       <c r="B27" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" t="s">
         <v>75</v>
-      </c>
-      <c r="C27" t="s">
-        <v>76</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -2498,10 +2500,10 @@
         <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C28" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -2512,7 +2514,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="19">
         <f>SUM(E7:E28)</f>
@@ -2521,12 +2523,12 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A32" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
@@ -2581,17 +2583,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="B6" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2602,13 +2604,13 @@
         <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3063,7 +3065,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E33" s="21">
         <f>SUM(E8:E32)</f>
@@ -3097,12 +3099,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3113,13 +3115,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>29</v>
@@ -3177,10 +3179,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3203,7 +3205,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D13" s="3">
         <v>21</v>
@@ -3221,7 +3223,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3238,37 +3240,37 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3279,7 +3281,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -3668,13 +3670,13 @@
       </c>
       <c r="B46" s="31"/>
       <c r="C46" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D46" s="31">
         <v>6</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -3686,7 +3688,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" s="1"/>
@@ -3697,21 +3699,21 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Uodated missing links on pdf
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="341" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A4853933-9075-4FD1-8E42-3FACC9A9FEE0}"/>
+  <xr:revisionPtr revIDLastSave="350" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A0D90DEF-DAD7-43E5-B4FE-ED3FD661B391}"/>
   <bookViews>
-    <workbookView xWindow="26208" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27156" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -616,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -672,6 +672,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1781,46 +1782,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
@@ -2085,7 +2086,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2571,7 +2572,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A389EA4-5A5F-4A9C-B048-2EB9BC969CA3}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2851,7 +2854,7 @@
       <c r="A21" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="37" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="11">
@@ -2869,7 +2872,7 @@
       <c r="A22" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="37" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="12">
@@ -2887,7 +2890,7 @@
       <c r="A23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="37" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="11">
@@ -3073,9 +3076,14 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B23" r:id="rId1" xr:uid="{9C45EC9D-EFBE-4139-AE55-A51B530AEB2B}"/>
+    <hyperlink ref="B22" r:id="rId2" xr:uid="{F9FAED66-AE20-478E-8EDC-73ACBB086917}"/>
+    <hyperlink ref="B21" r:id="rId3" xr:uid="{6B5BFB33-3A2C-4905-A9FF-9CDA02CFE35B}"/>
+  </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -3086,7 +3094,7 @@
   </sheetPr>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A38" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
added links to the fastener bom list
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="350" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{A0D90DEF-DAD7-43E5-B4FE-ED3FD661B391}"/>
+  <xr:revisionPtr revIDLastSave="371" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{E2818071-AB75-4678-B774-3E6A6D7C9F7C}"/>
   <bookViews>
-    <workbookView xWindow="27156" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27156" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="146">
   <si>
     <t>Part Name</t>
   </si>
@@ -474,6 +474,9 @@
   </si>
   <si>
     <t>Clone Price</t>
+  </si>
+  <si>
+    <t>DIN 7991</t>
   </si>
 </sst>
 </file>
@@ -672,7 +675,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2085,8 +2088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2572,9 +2575,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A389EA4-5A5F-4A9C-B048-2EB9BC969CA3}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2851,10 +2852,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="31" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="11">
@@ -2869,10 +2870,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="37" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="31" t="s">
         <v>40</v>
       </c>
       <c r="C22" s="12">
@@ -2887,10 +2888,10 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="31" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="11">
@@ -3049,11 +3050,11 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="11" t="s">
-        <v>45</v>
+      <c r="B32" s="31" t="s">
+        <v>145</v>
       </c>
       <c r="C32" s="12">
         <v>25</v>
@@ -3077,13 +3078,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B23" r:id="rId1" xr:uid="{9C45EC9D-EFBE-4139-AE55-A51B530AEB2B}"/>
-    <hyperlink ref="B22" r:id="rId2" xr:uid="{F9FAED66-AE20-478E-8EDC-73ACBB086917}"/>
-    <hyperlink ref="B21" r:id="rId3" xr:uid="{6B5BFB33-3A2C-4905-A9FF-9CDA02CFE35B}"/>
+    <hyperlink ref="A32" r:id="rId1" xr:uid="{EF3745AA-0BDE-4ACE-ACA4-B7BF3318EC84}"/>
+    <hyperlink ref="A21" r:id="rId2" xr:uid="{CF5CFF92-34AA-4B36-BDCF-7DF4689336D3}"/>
+    <hyperlink ref="A22" r:id="rId3" xr:uid="{E7E2016D-6DD4-45CC-91C0-B368A8D5C40A}"/>
+    <hyperlink ref="A23" r:id="rId4" xr:uid="{709D6F74-EB97-4B6F-BBEB-E00F1AB7877F}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated some links and a groove mount for the titan
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="377" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9569E0A5-071F-493C-8661-9E38B88A5548}"/>
+  <xr:revisionPtr revIDLastSave="394" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5616F7C7-20D3-4F96-91BD-2C9437C993C5}"/>
   <bookViews>
-    <workbookView xWindow="27156" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27156" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
   <si>
     <t>Part Name</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>DIN 7991</t>
+  </si>
+  <si>
+    <t>24V to 12V DC Converter</t>
+  </si>
+  <si>
+    <t>1.5A 18W DC DC Converter</t>
   </si>
 </sst>
 </file>
@@ -1087,9 +1093,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>15240</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1854,7 +1860,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="27">
-        <f>'Component Part List'!E29</f>
+        <f>'Component Part List'!E30</f>
         <v>295</v>
       </c>
     </row>
@@ -1912,7 +1918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{351499B6-19B9-45E8-927B-68CCDCB89EE0}">
   <dimension ref="A5:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2086,15 +2094,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -2515,26 +2525,41 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="18"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E30" s="19">
         <f>SUM(E7:E28)</f>
         <v>295</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A32" s="7" t="s">
+    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="A33" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="4"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C38" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2562,10 +2587,11 @@
     <hyperlink ref="B25" r:id="rId22" xr:uid="{42695F20-A1CA-4BFF-B93A-3229A8617449}"/>
     <hyperlink ref="C20" r:id="rId23" display="e3d Type Hotend" xr:uid="{E84D0B7A-20D8-46FC-A33D-C20E4015FB33}"/>
     <hyperlink ref="B20" r:id="rId24" display="J-Head/E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
+    <hyperlink ref="B29" r:id="rId25" display="24V to 12V 1.5A 18W DC Converter" xr:uid="{8579414B-CAF8-4100-8876-59E8317ACCBE}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
-  <drawing r:id="rId26"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <drawing r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -2573,9 +2599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A389EA4-5A5F-4A9C-B048-2EB9BC969CA3}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>

<commit_message>
added som driver links to bom
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="394" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{5616F7C7-20D3-4F96-91BD-2C9437C993C5}"/>
+  <xr:revisionPtr revIDLastSave="407" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7C1D8ACC-9113-4810-8269-F21CC90174E9}"/>
   <bookViews>
     <workbookView xWindow="27156" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="150">
   <si>
     <t>Part Name</t>
   </si>
@@ -257,9 +257,6 @@
     <t>DRV 8825</t>
   </si>
   <si>
-    <t>Stepper Drivers</t>
-  </si>
-  <si>
     <t>12864 LCD</t>
   </si>
   <si>
@@ -483,6 +480,15 @@
   </si>
   <si>
     <t>1.5A 18W DC DC Converter</t>
+  </si>
+  <si>
+    <t>TMC2208</t>
+  </si>
+  <si>
+    <t>XY Stepper Drivers</t>
+  </si>
+  <si>
+    <t>ZE Stepper Drivers</t>
   </si>
 </sst>
 </file>
@@ -1792,7 +1798,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
       <c r="A1" s="38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1806,7 +1812,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1820,7 +1826,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -1848,7 +1854,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B6" s="27">
         <f>'V-Slots and Wheels List'!F17</f>
@@ -1857,16 +1863,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="27">
-        <f>'Component Part List'!E30</f>
-        <v>295</v>
+        <f>'Component Part List'!E31</f>
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="27">
         <f>'Fasteners List'!E33</f>
@@ -1879,21 +1885,21 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
-        <v>543</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A13" s="25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1933,10 +1939,10 @@
   <sheetData>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
         <v>130</v>
-      </c>
-      <c r="D5" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1951,10 +1957,10 @@
         <v>2</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -2043,7 +2049,7 @@
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D15" s="3">
         <v>21</v>
@@ -2065,7 +2071,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
@@ -2074,12 +2080,12 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A20" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -2094,11 +2100,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2112,12 +2116,12 @@
     <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -2131,10 +2135,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F6" s="15"/>
     </row>
@@ -2163,7 +2167,7 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2180,7 +2184,7 @@
         <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -2191,10 +2195,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
@@ -2209,10 +2213,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>65</v>
@@ -2226,13 +2230,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -2243,13 +2247,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
         <v>92</v>
-      </c>
-      <c r="C13" t="s">
-        <v>93</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2280,10 +2284,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -2298,10 +2302,10 @@
         <v>61</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2315,10 +2319,10 @@
         <v>61</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
         <v>79</v>
-      </c>
-      <c r="C17" t="s">
-        <v>80</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2367,10 +2371,10 @@
         <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>140</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>141</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2379,7 +2383,7 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2387,10 +2391,10 @@
         <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2399,7 +2403,7 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2407,19 +2411,19 @@
         <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" s="22">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2427,7 +2431,7 @@
         <v>69</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -2444,16 +2448,16 @@
         <v>69</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>148</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="18">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2461,50 +2465,50 @@
         <v>69</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>149</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E25" s="18">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>87</v>
+      <c r="B26" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>73</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" s="18">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C27" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" s="18">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2512,16 +2516,16 @@
         <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>138</v>
+        <v>74</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2529,37 +2533,56 @@
         <v>61</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="18">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="E30" s="19">
-        <f>SUM(E7:E28)</f>
-        <v>295</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C30" t="s">
+        <v>146</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="19">
+        <f>SUM(E7:E30)</f>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.75">
+      <c r="A34" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A33" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="4"/>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C39" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2571,10 +2594,10 @@
     <hyperlink ref="B14" r:id="rId6" xr:uid="{94C4C13B-0BBB-4F7B-A730-B3205BF6E8ED}"/>
     <hyperlink ref="B23" r:id="rId7" xr:uid="{36DCFF59-08CA-412B-82D6-7AAD9283F4CA}"/>
     <hyperlink ref="B21" r:id="rId8" xr:uid="{BB4FD47C-E877-4261-A969-740DE1E39AB4}"/>
-    <hyperlink ref="B27" r:id="rId9" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
+    <hyperlink ref="B28" r:id="rId9" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
     <hyperlink ref="B17" r:id="rId10" xr:uid="{13ECE8A0-6EE8-4028-9765-E96A93DC6FCD}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{2A7E1508-6E65-4E26-BF99-CF81B8D345E1}"/>
-    <hyperlink ref="B26" r:id="rId12" xr:uid="{25020B41-41DF-478E-89B1-FE4B385546EA}"/>
+    <hyperlink ref="B27" r:id="rId12" xr:uid="{25020B41-41DF-478E-89B1-FE4B385546EA}"/>
     <hyperlink ref="B19" r:id="rId13" xr:uid="{94831F77-CC8B-4258-8675-6442526C91B3}"/>
     <hyperlink ref="B12" r:id="rId14" xr:uid="{007564D3-D88A-459E-82C7-E7C8214C723F}"/>
     <hyperlink ref="B13" r:id="rId15" xr:uid="{4B39742A-81FB-4551-BEF4-69D5B4E51D2B}"/>
@@ -2582,16 +2605,17 @@
     <hyperlink ref="B22" r:id="rId17" display="BL Touch Probe" xr:uid="{4921FFD9-8616-4796-AF0F-67C77EA5A27C}"/>
     <hyperlink ref="C22" r:id="rId18" xr:uid="{D8FBE80D-6647-42BD-AA31-6FB3B8A2D48A}"/>
     <hyperlink ref="C21" r:id="rId19" xr:uid="{55B76075-89E5-4B66-9E0E-72A33EE17BD5}"/>
-    <hyperlink ref="B28" r:id="rId20" xr:uid="{20CA74F6-9B49-4A6D-8DB6-16AFDE7D4641}"/>
-    <hyperlink ref="B24" r:id="rId21" xr:uid="{B94573F1-B78C-47F1-B3ED-C228D2514D12}"/>
-    <hyperlink ref="B25" r:id="rId22" xr:uid="{42695F20-A1CA-4BFF-B93A-3229A8617449}"/>
+    <hyperlink ref="B29" r:id="rId20" xr:uid="{20CA74F6-9B49-4A6D-8DB6-16AFDE7D4641}"/>
+    <hyperlink ref="B25" r:id="rId21" xr:uid="{B94573F1-B78C-47F1-B3ED-C228D2514D12}"/>
+    <hyperlink ref="B26" r:id="rId22" xr:uid="{42695F20-A1CA-4BFF-B93A-3229A8617449}"/>
     <hyperlink ref="C20" r:id="rId23" display="e3d Type Hotend" xr:uid="{E84D0B7A-20D8-46FC-A33D-C20E4015FB33}"/>
     <hyperlink ref="B20" r:id="rId24" display="J-Head/E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
-    <hyperlink ref="B29" r:id="rId25" display="24V to 12V 1.5A 18W DC Converter" xr:uid="{8579414B-CAF8-4100-8876-59E8317ACCBE}"/>
+    <hyperlink ref="B30" r:id="rId25" display="24V to 12V 1.5A 18W DC Converter" xr:uid="{8579414B-CAF8-4100-8876-59E8317ACCBE}"/>
+    <hyperlink ref="B24" r:id="rId26" xr:uid="{4DC07155-221F-4F7E-8AAF-0772C9665106}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
-  <drawing r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <drawing r:id="rId28"/>
 </worksheet>
 </file>
 
@@ -2611,17 +2635,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="B6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -2632,13 +2656,13 @@
         <v>29</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -3078,7 +3102,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C32" s="12">
         <v>25</v>
@@ -3093,7 +3117,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E33" s="21">
         <f>SUM(E8:E32)</f>
@@ -3133,12 +3157,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -3149,13 +3173,13 @@
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>29</v>
@@ -3213,10 +3237,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3239,7 +3263,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D13" s="3">
         <v>21</v>
@@ -3257,7 +3281,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
@@ -3274,37 +3298,37 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -3315,7 +3339,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -3704,13 +3728,13 @@
       </c>
       <c r="B46" s="31"/>
       <c r="C46" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D46" s="31">
         <v>6</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -3722,7 +3746,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" s="1"/>
@@ -3733,21 +3757,21 @@
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fan link in bom
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="421" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{9053C31A-34D4-40D5-9369-8FBEB744956E}"/>
+  <xr:revisionPtr revIDLastSave="432" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{B3E0EC83-48AA-4AB5-8BF2-1C32DA99CF8E}"/>
   <bookViews>
-    <workbookView xWindow="27156" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28080" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="149">
   <si>
     <t>Part Name</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Thoothed Motor Pulley</t>
   </si>
   <si>
-    <t>GT2 Idler Pulley 20NT</t>
-  </si>
-  <si>
     <t>GT2 Idler Pulley 20T</t>
   </si>
   <si>
@@ -467,21 +464,12 @@
     <t>5mm X 555 mm Steel rod</t>
   </si>
   <si>
-    <t>12V Layer Fan</t>
-  </si>
-  <si>
     <t>Clone Price</t>
   </si>
   <si>
     <t>DIN 7991</t>
   </si>
   <si>
-    <t>24V to 12V DC Converter</t>
-  </si>
-  <si>
-    <t>1.5A 18W DC DC Converter</t>
-  </si>
-  <si>
     <t>TMC2208</t>
   </si>
   <si>
@@ -489,6 +477,15 @@
   </si>
   <si>
     <t>ZE Stepper Drivers</t>
+  </si>
+  <si>
+    <t>1.7A Nema 17 Stepper Motor</t>
+  </si>
+  <si>
+    <t>GT2 Idler Pulley Smooth</t>
+  </si>
+  <si>
+    <t>12/24V Layer Fan</t>
   </si>
 </sst>
 </file>
@@ -1790,15 +1787,15 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1810,9 +1807,9 @@
       <c r="I1" s="38"/>
       <c r="J1" s="38"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B2" s="39"/>
       <c r="C2" s="39"/>
@@ -1824,9 +1821,9 @@
       <c r="I2" s="39"/>
       <c r="J2" s="39"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -1838,66 +1835,66 @@
       <c r="I3" s="40"/>
       <c r="J3" s="40"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B6" s="27">
         <f>'V-Slots and Wheels List'!F17</f>
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="27">
+        <f>'Component Part List'!E30</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B7" s="27">
-        <f>'Component Part List'!E31</f>
-        <v>317</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="B8" s="27">
         <f>'Fasteners List'!E33</f>
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="27"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
-        <v>565</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29.25" x14ac:dyDescent="0.6">
       <c r="A13" s="25" t="s">
         <v>77</v>
       </c>
@@ -1928,24 +1925,24 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C5" s="33" t="s">
+        <v>128</v>
+      </c>
+      <c r="D5" t="s">
         <v>129</v>
       </c>
-      <c r="D5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>0</v>
       </c>
@@ -1960,10 +1957,10 @@
         <v>85</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1971,7 +1968,7 @@
       <c r="C8" s="1"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1990,7 +1987,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -2009,7 +2006,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -2028,14 +2025,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="33"/>
       <c r="E13" s="34"/>
       <c r="F13" s="35"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -2044,12 +2041,12 @@
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D15" s="3">
         <v>21</v>
@@ -2062,28 +2059,28 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="D16" s="3"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F17" s="23">
         <f>SUM(F10:F15)</f>
         <v>172</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:6" ht="29.25" x14ac:dyDescent="0.6">
       <c r="A20" s="7" t="s">
         <v>77</v>
       </c>
@@ -2100,31 +2097,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050CE5BC-D89A-4220-843F-C276095034F7}">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.600000000000001" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
@@ -2142,7 +2139,7 @@
       </c>
       <c r="F6" s="15"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -2159,7 +2156,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -2167,7 +2164,7 @@
         <v>64</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2176,7 +2173,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -2193,12 +2190,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
@@ -2211,12 +2208,12 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>88</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
         <v>65</v>
@@ -2228,12 +2225,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
         <v>87</v>
@@ -2245,15 +2242,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" t="s">
         <v>91</v>
-      </c>
-      <c r="C13" t="s">
-        <v>92</v>
       </c>
       <c r="D13">
         <v>10</v>
@@ -2262,7 +2259,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -2279,15 +2276,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="D15">
         <v>20</v>
@@ -2297,7 +2294,7 @@
       </c>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>61</v>
       </c>
@@ -2305,7 +2302,7 @@
         <v>84</v>
       </c>
       <c r="C16" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2314,7 +2311,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>61</v>
       </c>
@@ -2331,7 +2328,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>61</v>
       </c>
@@ -2348,33 +2345,33 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>11</v>
+        <v>146</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E19" s="18">
         <v>40</v>
       </c>
       <c r="F19" s="16"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>140</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2383,18 +2380,18 @@
         <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>61</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -2403,18 +2400,18 @@
         <v>20</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -2423,15 +2420,15 @@
         <v>15</v>
       </c>
       <c r="F22" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -2443,15 +2440,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -2460,7 +2457,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>69</v>
       </c>
@@ -2468,16 +2465,16 @@
         <v>71</v>
       </c>
       <c r="C25" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E25" s="18">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>69</v>
       </c>
@@ -2494,7 +2491,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>69</v>
       </c>
@@ -2511,12 +2508,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C28" t="s">
         <v>74</v>
@@ -2525,18 +2522,18 @@
         <v>1</v>
       </c>
       <c r="E28" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>61</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" t="s">
         <v>136</v>
-      </c>
-      <c r="C29" t="s">
-        <v>137</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -2545,44 +2542,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C30" t="s">
-        <v>146</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" s="19">
-        <f>SUM(E7:E30)</f>
-        <v>317</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="E30" s="19">
+        <f>SUM(E7:E29)</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="A34" s="7" t="s">
+    <row r="33" spans="1:3" ht="29.25" x14ac:dyDescent="0.6">
+      <c r="A33" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="4"/>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2590,11 +2570,11 @@
     <hyperlink ref="B16" r:id="rId2" xr:uid="{3CEA6465-8B09-4BC6-B69F-5E20C6200862}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{815E5D15-CF78-41EC-980C-BB8E5720E054}"/>
     <hyperlink ref="B10" r:id="rId4" xr:uid="{B148155D-7B0C-4B5A-A63D-846513AC87D8}"/>
-    <hyperlink ref="B11" r:id="rId5" xr:uid="{0BA4E21B-2D6F-419E-BB1C-022ED717A36F}"/>
+    <hyperlink ref="B11" r:id="rId5" display="GT2 Idler Pulley 20NT" xr:uid="{0BA4E21B-2D6F-419E-BB1C-022ED717A36F}"/>
     <hyperlink ref="B14" r:id="rId6" xr:uid="{94C4C13B-0BBB-4F7B-A730-B3205BF6E8ED}"/>
     <hyperlink ref="B23" r:id="rId7" xr:uid="{36DCFF59-08CA-412B-82D6-7AAD9283F4CA}"/>
     <hyperlink ref="B21" r:id="rId8" xr:uid="{BB4FD47C-E877-4261-A969-740DE1E39AB4}"/>
-    <hyperlink ref="B28" r:id="rId9" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
+    <hyperlink ref="B28" r:id="rId9" display="12V Layer Fan" xr:uid="{CB297E9F-651F-4BC1-B041-888A78608872}"/>
     <hyperlink ref="B17" r:id="rId10" xr:uid="{13ECE8A0-6EE8-4028-9765-E96A93DC6FCD}"/>
     <hyperlink ref="B9" r:id="rId11" xr:uid="{2A7E1508-6E65-4E26-BF99-CF81B8D345E1}"/>
     <hyperlink ref="B27" r:id="rId12" xr:uid="{25020B41-41DF-478E-89B1-FE4B385546EA}"/>
@@ -2609,13 +2589,12 @@
     <hyperlink ref="B26" r:id="rId21" xr:uid="{42695F20-A1CA-4BFF-B93A-3229A8617449}"/>
     <hyperlink ref="C20" r:id="rId22" display="e3d Type Hotend" xr:uid="{E84D0B7A-20D8-46FC-A33D-C20E4015FB33}"/>
     <hyperlink ref="B20" r:id="rId23" display="J-Head/E3d Hotend" xr:uid="{D9CC2680-375C-425C-9B23-A84445726301}"/>
-    <hyperlink ref="B30" r:id="rId24" display="24V to 12V 1.5A 18W DC Converter" xr:uid="{8579414B-CAF8-4100-8876-59E8317ACCBE}"/>
-    <hyperlink ref="B24" r:id="rId25" xr:uid="{4DC07155-221F-4F7E-8AAF-0772C9665106}"/>
-    <hyperlink ref="B19" r:id="rId26" xr:uid="{94831F77-CC8B-4258-8675-6442526C91B3}"/>
+    <hyperlink ref="B24" r:id="rId24" xr:uid="{4DC07155-221F-4F7E-8AAF-0772C9665106}"/>
+    <hyperlink ref="B19" r:id="rId25" display="Nema 17 Stepper Motor" xr:uid="{94831F77-CC8B-4258-8675-6442526C91B3}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
-  <drawing r:id="rId28"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
+  <drawing r:id="rId27"/>
 </worksheet>
 </file>
 
@@ -2625,30 +2604,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:5" ht="29.25" x14ac:dyDescent="0.6">
       <c r="B6" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>46</v>
       </c>
@@ -2659,13 +2638,13 @@
         <v>81</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>22</v>
       </c>
@@ -2683,7 +2662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -2701,7 +2680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>13</v>
       </c>
@@ -2719,7 +2698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>50</v>
       </c>
@@ -2737,7 +2716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
@@ -2755,7 +2734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>14</v>
       </c>
@@ -2773,7 +2752,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>57</v>
       </c>
@@ -2791,7 +2770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>19</v>
       </c>
@@ -2809,7 +2788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>24</v>
       </c>
@@ -2827,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
@@ -2845,7 +2824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>36</v>
       </c>
@@ -2863,7 +2842,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>17</v>
       </c>
@@ -2881,7 +2860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>38</v>
       </c>
@@ -2899,7 +2878,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>47</v>
       </c>
@@ -2917,7 +2896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
         <v>39</v>
       </c>
@@ -2935,7 +2914,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>7</v>
       </c>
@@ -2953,7 +2932,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>9</v>
       </c>
@@ -2971,7 +2950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>10</v>
       </c>
@@ -2989,7 +2968,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>41</v>
       </c>
@@ -3007,7 +2986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>42</v>
       </c>
@@ -3025,7 +3004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>25</v>
       </c>
@@ -3043,7 +3022,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>18</v>
       </c>
@@ -3061,7 +3040,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>15</v>
       </c>
@@ -3079,7 +3058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>44</v>
       </c>
@@ -3097,12 +3076,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C32" s="12">
         <v>25</v>
@@ -3115,9 +3094,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E33" s="21">
         <f>SUM(E8:E32)</f>
@@ -3146,34 +3125,34 @@
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>1</v>
@@ -3185,7 +3164,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -3193,7 +3172,7 @@
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -3207,7 +3186,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -3221,7 +3200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -3235,12 +3214,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="D11">
         <v>16</v>
@@ -3249,7 +3228,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -3257,13 +3236,13 @@
       <c r="C12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D13" s="3">
         <v>21</v>
@@ -3272,21 +3251,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="3"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -3298,48 +3277,48 @@
         <v>4</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D17">
         <v>10</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18">
         <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="2" t="s">
@@ -3347,7 +3326,7 @@
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
         <v>22</v>
       </c>
@@ -3362,7 +3341,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
         <v>16</v>
       </c>
@@ -3377,7 +3356,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
         <v>13</v>
       </c>
@@ -3392,7 +3371,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
         <v>50</v>
       </c>
@@ -3407,7 +3386,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="31" t="s">
         <v>21</v>
       </c>
@@ -3422,7 +3401,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="31" t="s">
         <v>14</v>
       </c>
@@ -3437,7 +3416,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="31" t="s">
         <v>57</v>
       </c>
@@ -3452,7 +3431,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="31" t="s">
         <v>19</v>
       </c>
@@ -3467,7 +3446,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="31" t="s">
         <v>24</v>
       </c>
@@ -3482,7 +3461,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="31" t="s">
         <v>23</v>
       </c>
@@ -3497,7 +3476,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="31" t="s">
         <v>36</v>
       </c>
@@ -3512,7 +3491,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="31" t="s">
         <v>17</v>
       </c>
@@ -3527,7 +3506,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="31" t="s">
         <v>38</v>
       </c>
@@ -3542,7 +3521,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="31" t="s">
         <v>47</v>
       </c>
@@ -3557,7 +3536,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="31" t="s">
         <v>39</v>
       </c>
@@ -3572,7 +3551,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="s">
         <v>7</v>
       </c>
@@ -3587,7 +3566,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="s">
         <v>9</v>
       </c>
@@ -3602,7 +3581,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="s">
         <v>10</v>
       </c>
@@ -3617,7 +3596,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="s">
         <v>41</v>
       </c>
@@ -3632,7 +3611,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="31" t="s">
         <v>42</v>
       </c>
@@ -3647,7 +3626,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="31" t="s">
         <v>25</v>
       </c>
@@ -3662,7 +3641,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="31" t="s">
         <v>18</v>
       </c>
@@ -3677,7 +3656,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="31" t="s">
         <v>15</v>
       </c>
@@ -3692,7 +3671,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="31" t="s">
         <v>44</v>
       </c>
@@ -3707,7 +3686,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="31" t="s">
         <v>31</v>
       </c>
@@ -3722,51 +3701,51 @@
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="31" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="31"/>
       <c r="C46" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D46" s="31">
         <v>6</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="31"/>
       <c r="C47" s="31"/>
       <c r="D47" s="31"/>
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C48" s="2"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="29.25" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
         <v>76</v>
       </c>

</xml_diff>

<commit_message>
small name changes and simplifying
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="600" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{BE48EB62-67C3-45E6-8768-EAD354C73A6C}"/>
+  <xr:revisionPtr revIDLastSave="634" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{55444F7A-269D-444E-A65D-BF0F11778B79}"/>
   <bookViews>
-    <workbookView xWindow="28080" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29010" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="124">
   <si>
     <t>Part Name</t>
   </si>
@@ -78,9 +78,6 @@
     <t>M3 NUT</t>
   </si>
   <si>
-    <t>M5 Nut</t>
-  </si>
-  <si>
     <t>M5x30</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>M3X25</t>
   </si>
   <si>
-    <t>M3 Lock Nut</t>
-  </si>
-  <si>
     <t>M4x20</t>
   </si>
   <si>
@@ -120,21 +114,9 @@
     <t>M5x8 Countersink</t>
   </si>
   <si>
-    <t>Nylon Lock Nut M3</t>
-  </si>
-  <si>
     <t>Standard Nut M5</t>
   </si>
   <si>
-    <t>M5 Nut lock</t>
-  </si>
-  <si>
-    <t>M5 T-Nut Open Builds</t>
-  </si>
-  <si>
-    <t>OpenBuilds Tee Nut M5</t>
-  </si>
-  <si>
     <t>M5x12</t>
   </si>
   <si>
@@ -399,12 +381,6 @@
     <t>Bulk Quantity</t>
   </si>
   <si>
-    <t>M5 Wheel Shim</t>
-  </si>
-  <si>
-    <t>Precision Shim for V-Slot Big Wheels</t>
-  </si>
-  <si>
     <t>Estimated Frame Kit Price</t>
   </si>
   <si>
@@ -412,6 +388,27 @@
   </si>
   <si>
     <t>No fasteners or cables included</t>
+  </si>
+  <si>
+    <t>M5 GT2 Idler Shim</t>
+  </si>
+  <si>
+    <t>Hex Locking Nut - M4</t>
+  </si>
+  <si>
+    <t>M4 Hex Nut lock</t>
+  </si>
+  <si>
+    <t>M5 Hex Nut</t>
+  </si>
+  <si>
+    <t>M5 Hex Nut lock</t>
+  </si>
+  <si>
+    <t>Precision Shim for GT2 idlers/pulleys</t>
+  </si>
+  <si>
+    <t>Cables</t>
   </si>
 </sst>
 </file>
@@ -612,6 +609,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -621,7 +619,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1465,116 +1462,116 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B6" s="27">
         <f>'Complete Part List'!E15</f>
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B7" s="27">
         <f>'Complete Part List'!E39</f>
         <v>303</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B8" s="27">
-        <f>'Fasteners List'!E33</f>
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <f>'Fasteners List'!E32</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="27"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
-        <v>579</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A13" s="25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1599,40 +1596,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0919D6B9-0972-4CD2-93D2-3239C5F0D359}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="B1" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="35"/>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
@@ -1640,28 +1637,28 @@
         <v>1</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C7">
         <v>16</v>
@@ -1674,12 +1671,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1692,12 +1689,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -1710,12 +1707,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C10" s="1">
         <v>20</v>
@@ -1724,26 +1721,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="33"/>
       <c r="E11" s="16"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C13" s="3">
         <v>21</v>
@@ -1756,43 +1753,43 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="3"/>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="E15" s="23">
         <f>SUM(E7:E13)</f>
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1804,12 +1801,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1821,12 +1818,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1838,12 +1835,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1855,12 +1852,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1872,12 +1869,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1889,12 +1886,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C23" s="4">
         <v>1</v>
@@ -1906,12 +1903,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1923,12 +1920,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C25">
         <v>8</v>
@@ -1940,12 +1937,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -1957,12 +1954,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -1974,12 +1971,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -1991,12 +1988,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="C29" s="4">
         <v>1</v>
@@ -2008,12 +2005,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -2025,12 +2022,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C31" s="9">
         <v>1</v>
@@ -2042,12 +2039,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="C32" s="9">
         <v>1</v>
@@ -2059,12 +2056,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C33" s="4">
         <v>1</v>
@@ -2076,12 +2073,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="C34" s="9">
         <v>1</v>
@@ -2093,12 +2090,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C35" s="9">
         <v>1</v>
@@ -2110,9 +2107,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>8</v>
@@ -2127,12 +2124,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B37" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C37" s="9">
         <v>1</v>
@@ -2144,12 +2141,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C38" s="9">
         <v>1</v>
@@ -2161,27 +2158,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E39" s="19">
         <f>SUM(E17:E38)</f>
         <v>303</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="39">
+        <v>115</v>
+      </c>
+      <c r="E41" s="36">
         <f>E39+E15</f>
         <v>503</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2224,166 +2221,164 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A389EA4-5A5F-4A9C-B048-2EB9BC969CA3}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="25.5" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="12">
-        <v>10</v>
+        <v>39</v>
+      </c>
+      <c r="C8" s="11">
+        <v>25</v>
       </c>
       <c r="D8" s="32">
         <v>0.1</v>
       </c>
       <c r="E8" s="31">
         <f>D8*C8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="11">
-        <v>10</v>
+        <v>38</v>
+      </c>
+      <c r="C9" s="12">
+        <v>25</v>
       </c>
       <c r="D9" s="32">
         <v>0.1</v>
       </c>
       <c r="E9" s="31">
-        <f t="shared" ref="E9:E32" si="0">D9*C9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D9*C9</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="12">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="11">
+        <v>25</v>
       </c>
       <c r="D10" s="32">
         <v>0.1</v>
       </c>
       <c r="E10" s="31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D10*C10</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="11">
+        <v>16</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="12">
         <v>10</v>
       </c>
       <c r="D11" s="32">
         <v>0.1</v>
       </c>
       <c r="E11" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D11*C11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="11">
         <v>25</v>
-      </c>
-      <c r="C12" s="12">
-        <v>10</v>
       </c>
       <c r="D12" s="32">
         <v>0.1</v>
       </c>
       <c r="E12" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D12*C12</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="12">
         <v>10</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="11">
-        <v>20</v>
       </c>
       <c r="D13" s="32">
         <v>0.1</v>
       </c>
       <c r="E13" s="31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D13*C13</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="C14" s="12">
         <v>10</v>
@@ -2392,16 +2387,16 @@
         <v>0.1</v>
       </c>
       <c r="E14" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D14*C14</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C15" s="11">
         <v>10</v>
@@ -2410,16 +2405,16 @@
         <v>0.1</v>
       </c>
       <c r="E15" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D15*C15</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C16" s="12">
         <v>10</v>
@@ -2428,16 +2423,16 @@
         <v>0.1</v>
       </c>
       <c r="E16" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D16*C16</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="11">
         <v>10</v>
@@ -2446,34 +2441,34 @@
         <v>0.1</v>
       </c>
       <c r="E17" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D17*C17</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C18" s="12">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="D18" s="32">
         <v>0.1</v>
       </c>
       <c r="E18" s="31">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D18*C18</f>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>13</v>
+        <v>120</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C19" s="11">
         <v>20</v>
@@ -2482,16 +2477,16 @@
         <v>0.1</v>
       </c>
       <c r="E19" s="31">
-        <f t="shared" si="0"/>
+        <f>D19*C19</f>
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C20" s="12">
         <v>40</v>
@@ -2500,16 +2495,16 @@
         <v>0.1</v>
       </c>
       <c r="E20" s="31">
-        <f t="shared" si="0"/>
+        <f>D20*C20</f>
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C21" s="11">
         <v>50</v>
@@ -2518,227 +2513,228 @@
         <v>0.1</v>
       </c>
       <c r="E21" s="31">
-        <f t="shared" si="0"/>
+        <f>D21*C21</f>
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="34" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="12">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="C22" s="11">
+        <v>100</v>
       </c>
       <c r="D22" s="32">
         <v>0.1</v>
       </c>
       <c r="E22" s="31">
-        <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="11">
-        <v>75</v>
+        <f>D22*C22</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="12">
+        <v>150</v>
       </c>
       <c r="D23" s="32">
         <v>0.1</v>
       </c>
       <c r="E23" s="31">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D23*C23</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C24" s="12">
-        <v>150</v>
+        <v>23</v>
+      </c>
+      <c r="C24" s="11">
+        <v>100</v>
       </c>
       <c r="D24" s="32">
         <v>0.1</v>
       </c>
       <c r="E24" s="31">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D24*C24</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="11">
-        <v>100</v>
+        <v>23</v>
+      </c>
+      <c r="C25" s="12">
+        <v>10</v>
       </c>
       <c r="D25" s="32">
         <v>0.1</v>
       </c>
       <c r="E25" s="31">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D25*C25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="12">
-        <v>10</v>
+        <v>28</v>
+      </c>
+      <c r="C26" s="11">
+        <v>20</v>
       </c>
       <c r="D26" s="32">
         <v>0.1</v>
       </c>
       <c r="E26" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D26*C26</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="11">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C27" s="12">
+        <v>10</v>
       </c>
       <c r="D27" s="32">
         <v>0.1</v>
       </c>
       <c r="E27" s="31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D27*C27</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="12">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="C28" s="11">
+        <v>20</v>
       </c>
       <c r="D28" s="32">
         <v>0.1</v>
       </c>
       <c r="E28" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D28*C28</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="11">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C29" s="12">
+        <v>10</v>
       </c>
       <c r="D29" s="32">
         <v>0.1</v>
       </c>
       <c r="E29" s="31">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <f>D29*C29</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="12">
+        <v>28</v>
+      </c>
+      <c r="C30" s="11">
         <v>10</v>
       </c>
       <c r="D30" s="32">
         <v>0.1</v>
       </c>
       <c r="E30" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="11">
-        <v>10</v>
+        <f>D30*C30</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="12">
+        <v>25</v>
       </c>
       <c r="D31" s="32">
         <v>0.1</v>
       </c>
       <c r="E31" s="31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C32" s="12">
-        <v>25</v>
-      </c>
-      <c r="D32" s="32">
-        <v>0.1</v>
-      </c>
-      <c r="E32" s="31">
-        <f t="shared" si="0"/>
+        <f>D31*C31</f>
         <v>2.5</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" s="21">
-        <f>SUM(E8:E32)</f>
-        <v>76</v>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="21">
+        <f>SUM(E8:E31)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A8:E31">
+    <sortCondition ref="A8:A31"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="A32" r:id="rId1" xr:uid="{EF3745AA-0BDE-4ACE-ACA4-B7BF3318EC84}"/>
-    <hyperlink ref="A22" r:id="rId2" xr:uid="{E7E2016D-6DD4-45CC-91C0-B368A8D5C40A}"/>
-    <hyperlink ref="A23" r:id="rId3" xr:uid="{709D6F74-EB97-4B6F-BBEB-E00F1AB7877F}"/>
-    <hyperlink ref="A21" r:id="rId4" xr:uid="{CF5CFF92-34AA-4B36-BDCF-7DF4689336D3}"/>
+    <hyperlink ref="A31" r:id="rId1" xr:uid="{EF3745AA-0BDE-4ACE-ACA4-B7BF3318EC84}"/>
+    <hyperlink ref="A22" r:id="rId2" xr:uid="{709D6F74-EB97-4B6F-BBEB-E00F1AB7877F}"/>
+    <hyperlink ref="A21" r:id="rId3" xr:uid="{CF5CFF92-34AA-4B36-BDCF-7DF4689336D3}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated zipfile in firmwares
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="651" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{A49060E9-6641-47C1-A06E-22369E86ECD2}"/>
+  <xr:revisionPtr revIDLastSave="658" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{5E94E7D2-CB85-427C-BCA9-099C1110E0B0}"/>
   <bookViews>
     <workbookView xWindow="29970" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="127">
   <si>
     <t>Part Name</t>
   </si>
@@ -507,13 +507,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,6 +522,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -577,7 +582,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -636,7 +641,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1632,12 +1639,14 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="40" t="s">
         <v>125</v>
       </c>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
     </row>
     <row r="5" spans="1:5" ht="29.25" x14ac:dyDescent="0.6">
       <c r="A5" s="35" t="s">
@@ -2227,7 +2236,7 @@
     <hyperlink ref="B24" r:id="rId18" xr:uid="{E10FFF22-2835-4984-B28A-963166E303EF}"/>
     <hyperlink ref="A33" r:id="rId19" xr:uid="{58DB2412-7C03-4A2F-9705-67EFFED8C1C0}"/>
     <hyperlink ref="A21" r:id="rId20" xr:uid="{0BB9972B-C050-4E02-969B-4ADA4E04C03C}"/>
-    <hyperlink ref="A31" r:id="rId21" display="12864 LCD" xr:uid="{CAE4404B-45D0-4E89-A4A3-4B25F59F94BE}"/>
+    <hyperlink ref="A31" r:id="rId21" xr:uid="{CAE4404B-45D0-4E89-A4A3-4B25F59F94BE}"/>
     <hyperlink ref="B30" r:id="rId22" display="e3d Type Hotend" xr:uid="{885939FD-E74B-47B9-BE71-B4231ABC303E}"/>
     <hyperlink ref="A30" r:id="rId23" display="J-Head/E3d Hotend" xr:uid="{81183C11-951E-4165-8179-AEB7A3753441}"/>
     <hyperlink ref="A22" r:id="rId24" display="TMC2208" xr:uid="{9DCE4818-32CB-4564-B0A5-F04B2E760BEC}"/>

</xml_diff>

<commit_message>
added worm gear rod link to BOM
</commit_message>
<xml_diff>
--- a/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
+++ b/Bill Of Materials/V-King PRO 400 Part Order List.xlsx
@@ -5,24 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roy\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Document Library\GitHub\V-King\Bill Of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="722" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{D7D09028-AF79-41C0-9D5C-3552F0BA831C}"/>
+  <xr:revisionPtr revIDLastSave="741" documentId="8_{BDB81E76-0EE6-4FBB-BB57-40CE6024A00A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{788C9825-6B78-49EA-8C3E-117D55956D5B}"/>
   <bookViews>
-    <workbookView xWindow="34728" yWindow="0" windowWidth="28800" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35670" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Overview" sheetId="7" r:id="rId1"/>
     <sheet name="Complete Part List" sheetId="10" r:id="rId2"/>
     <sheet name="Fasteners List" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -139,9 +138,6 @@
     <t>Drop In type Hammer Nut</t>
   </si>
   <si>
-    <t>Ball Bearing 5-16-5</t>
-  </si>
-  <si>
     <t>M3x10</t>
   </si>
   <si>
@@ -337,9 +333,6 @@
     <t>Fan - Layer Fan 12/24V</t>
   </si>
   <si>
-    <t>LCD - 12864 Controller</t>
-  </si>
-  <si>
     <t>Power Supply 24V</t>
   </si>
   <si>
@@ -412,9 +405,6 @@
     <t>V-King - Components to Buy</t>
   </si>
   <si>
-    <t>Machanical Kit+Fasteners here</t>
-  </si>
-  <si>
     <t>Component Part Name</t>
   </si>
   <si>
@@ -428,6 +418,15 @@
   </si>
   <si>
     <t>Fasteners included</t>
+  </si>
+  <si>
+    <t>Complete Kit</t>
+  </si>
+  <si>
+    <t>Controller LCD 12864</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5id-16od-5w Ball bearings</t>
   </si>
 </sst>
 </file>
@@ -650,6 +649,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -659,7 +659,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1503,116 +1502,116 @@
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="24" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.2" x14ac:dyDescent="0.45">
-      <c r="A1" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+    <row r="1" spans="1:10" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="41"/>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="41"/>
-      <c r="J3" s="41"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="6"/>
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
       <c r="E5" s="29"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="27">
         <f>'Complete Part List'!E14</f>
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="27">
         <f>'Complete Part List'!E39</f>
-        <v>355</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B8" s="27">
         <f>'Fasteners List'!E32</f>
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="27"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="26">
         <f>SUM(B6:B9)</f>
-        <v>630</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="29.25" x14ac:dyDescent="0.6">
       <c r="A13" s="25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1639,43 +1638,43 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.109375" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A1" s="5"/>
       <c r="B1" s="38" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="37" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D3" s="36"/>
       <c r="E3" s="36"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:5" ht="29.25" x14ac:dyDescent="0.6">
       <c r="A5" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
@@ -1683,28 +1682,30 @@
         <v>1</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="1"/>
+        <v>94</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>127</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8">
         <v>16</v>
@@ -1717,12 +1718,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1735,7 +1736,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>3</v>
       </c>
@@ -1753,12 +1754,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C11" s="1">
         <v>20</v>
@@ -1767,7 +1768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
@@ -1775,12 +1776,12 @@
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="3">
         <v>21</v>
@@ -1793,60 +1794,58 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>124</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="B14" s="13"/>
       <c r="E14" s="23">
         <f>SUM(E8:E13)</f>
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="E15" s="23"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B16" s="14"/>
       <c r="C16" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E17" s="18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -1855,12 +1854,12 @@
         <v>1</v>
       </c>
       <c r="E18" s="18">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
         <v>48</v>
@@ -1872,15 +1871,15 @@
         <v>1</v>
       </c>
       <c r="E19" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B20" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -1892,12 +1891,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1909,12 +1908,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1926,14 +1925,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="4">
+        <v>80</v>
+      </c>
+      <c r="C23">
         <v>1</v>
       </c>
       <c r="D23">
@@ -1943,12 +1942,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1960,12 +1959,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25">
         <v>8</v>
@@ -1977,12 +1976,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26">
         <v>10</v>
@@ -1994,12 +1993,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -2011,12 +2010,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
       </c>
       <c r="C28">
         <v>7</v>
@@ -2028,14 +2027,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C29" s="4">
+        <v>84</v>
+      </c>
+      <c r="C29">
         <v>1</v>
       </c>
       <c r="D29">
@@ -2045,224 +2044,225 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" s="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" s="22">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B30" t="s">
-        <v>49</v>
-      </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-      <c r="E30" s="18">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C31" s="9">
-        <v>1</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-      <c r="E31" s="18">
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" s="9">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33" s="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" s="9">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C35" s="9">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>4</v>
+      </c>
+      <c r="E35" s="18">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37">
+        <v>4</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+      <c r="E37" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>85</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" s="18">
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" s="18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33" s="4">
-        <v>1</v>
-      </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-      <c r="E33" s="22">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B34" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="9">
-        <v>1</v>
-      </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-      <c r="E35" s="18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="9">
-        <v>4</v>
-      </c>
-      <c r="D36">
-        <v>4</v>
-      </c>
-      <c r="E36" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" t="s">
-        <v>43</v>
-      </c>
-      <c r="C37" s="9">
-        <v>1</v>
-      </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" t="s">
-        <v>86</v>
-      </c>
-      <c r="C38" s="9">
-        <v>1</v>
-      </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-      <c r="E38" s="18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E39" s="19">
         <f>SUM(E17:E38)</f>
-        <v>355</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C42" t="s">
-        <v>129</v>
-      </c>
-      <c r="E42" s="42">
+        <v>126</v>
+      </c>
+      <c r="E42" s="39">
         <v>415</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:E38">
-    <sortCondition ref="A17"/>
+  <sortState ref="A17:E38">
+    <sortCondition ref="A17:A38"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="A22" r:id="rId1" display="Optical Sensor" xr:uid="{C32C274D-A6E0-4D8A-89C2-5039958B9192}"/>
-    <hyperlink ref="A34" r:id="rId2" display="350*400 Silicone Heatpad" xr:uid="{4CDCED05-F3FA-4EE2-9C5A-16C4111B5756}"/>
-    <hyperlink ref="A37" r:id="rId3" xr:uid="{CE3F6C39-A479-448C-AD14-3ED94A462295}"/>
+    <hyperlink ref="A33" r:id="rId2" display="350*400 Silicone Heatpad" xr:uid="{4CDCED05-F3FA-4EE2-9C5A-16C4111B5756}"/>
+    <hyperlink ref="A36" r:id="rId3" xr:uid="{CE3F6C39-A479-448C-AD14-3ED94A462295}"/>
     <hyperlink ref="A25" r:id="rId4" xr:uid="{9D4DEDA8-9BFB-4EFE-8A31-690877AB3F50}"/>
     <hyperlink ref="A26" r:id="rId5" display="GT2 Idler Pulley 20NT" xr:uid="{8B9E3E48-B339-4A1E-BBF7-47A80E28AA3C}"/>
-    <hyperlink ref="A18" r:id="rId6" display="Build Plate" xr:uid="{91CD28EF-6468-4F89-9D03-55545D2A7193}"/>
-    <hyperlink ref="A19" r:id="rId7" display="MKS Gen L V1.0" xr:uid="{05CE83E4-339D-45AB-BEE5-A57742852626}"/>
+    <hyperlink ref="A17" r:id="rId6" display="Build Plate" xr:uid="{91CD28EF-6468-4F89-9D03-55545D2A7193}"/>
+    <hyperlink ref="A18" r:id="rId7" display="MKS Gen L V1.0" xr:uid="{05CE83E4-339D-45AB-BEE5-A57742852626}"/>
     <hyperlink ref="A23" r:id="rId8" display="Filament Extruder" xr:uid="{2990F041-B107-435C-8E36-C6DB9AF434EE}"/>
     <hyperlink ref="A24" r:id="rId9" display="12V Layer Fan" xr:uid="{C0F4AF68-82D7-4FE3-85B1-F724D0E242E5}"/>
-    <hyperlink ref="A35" r:id="rId10" xr:uid="{8B08525D-D4AB-4388-990C-6264D12F7DD1}"/>
-    <hyperlink ref="A17" r:id="rId11" xr:uid="{5E9E73AA-5AF2-4E91-A648-438685B0C3D6}"/>
-    <hyperlink ref="A31" r:id="rId12" display="24V Power Supply" xr:uid="{4A606871-E536-40C8-BD7C-22C8F712CB42}"/>
+    <hyperlink ref="A34" r:id="rId10" xr:uid="{8B08525D-D4AB-4388-990C-6264D12F7DD1}"/>
+    <hyperlink ref="A37" r:id="rId11" display="Ball Bearing 5-16-5" xr:uid="{5E9E73AA-5AF2-4E91-A648-438685B0C3D6}"/>
+    <hyperlink ref="A30" r:id="rId12" display="24V Power Supply" xr:uid="{4A606871-E536-40C8-BD7C-22C8F712CB42}"/>
     <hyperlink ref="A28" r:id="rId13" xr:uid="{59CB82CB-DB6A-4646-8377-A6DDBB213953}"/>
     <hyperlink ref="A11" r:id="rId14" xr:uid="{62B72BE0-7647-4668-8FFD-AB380EEE8F6A}"/>
-    <hyperlink ref="A33" r:id="rId15" display="BL Touch Probe" xr:uid="{22CF7BD3-C320-4224-A2A9-6868041A199C}"/>
-    <hyperlink ref="B33" r:id="rId16" xr:uid="{FF98C7A6-1409-45CE-95A1-AA2FD51D9269}"/>
+    <hyperlink ref="A32" r:id="rId15" display="BL Touch Probe" xr:uid="{22CF7BD3-C320-4224-A2A9-6868041A199C}"/>
+    <hyperlink ref="B32" r:id="rId16" xr:uid="{FF98C7A6-1409-45CE-95A1-AA2FD51D9269}"/>
     <hyperlink ref="B23" r:id="rId17" xr:uid="{E10FFF22-2835-4984-B28A-963166E303EF}"/>
-    <hyperlink ref="A32" r:id="rId18" xr:uid="{58DB2412-7C03-4A2F-9705-67EFFED8C1C0}"/>
+    <hyperlink ref="A31" r:id="rId18" xr:uid="{58DB2412-7C03-4A2F-9705-67EFFED8C1C0}"/>
     <hyperlink ref="A20" r:id="rId19" xr:uid="{0BB9972B-C050-4E02-969B-4ADA4E04C03C}"/>
-    <hyperlink ref="A30" r:id="rId20" xr:uid="{CAE4404B-45D0-4E89-A4A3-4B25F59F94BE}"/>
+    <hyperlink ref="A19" r:id="rId20" display="LCD - 12864 Controller" xr:uid="{CAE4404B-45D0-4E89-A4A3-4B25F59F94BE}"/>
     <hyperlink ref="B29" r:id="rId21" display="e3d Type Hotend" xr:uid="{885939FD-E74B-47B9-BE71-B4231ABC303E}"/>
     <hyperlink ref="A29" r:id="rId22" display="J-Head/E3d Hotend" xr:uid="{81183C11-951E-4165-8179-AEB7A3753441}"/>
     <hyperlink ref="A21" r:id="rId23" display="TMC2208" xr:uid="{9DCE4818-32CB-4564-B0A5-F04B2E760BEC}"/>
-    <hyperlink ref="A36" r:id="rId24" display="Nema 17 Stepper Motor" xr:uid="{072E66F4-E1AF-417B-A243-668D51F20570}"/>
+    <hyperlink ref="A35" r:id="rId24" display="Nema 17 Stepper Motor" xr:uid="{072E66F4-E1AF-417B-A243-668D51F20570}"/>
     <hyperlink ref="C3" r:id="rId25" xr:uid="{29285AC2-32BB-4E9E-98C3-BEC5D34404E3}"/>
-    <hyperlink ref="B14" r:id="rId26" xr:uid="{A201CDB2-3052-42C4-B920-38638778A07F}"/>
-    <hyperlink ref="A13" r:id="rId27" xr:uid="{9833C20E-591F-42B7-828C-80D603985010}"/>
-    <hyperlink ref="A10" r:id="rId28" xr:uid="{F713CD95-16C8-4DB2-AAAF-F46DD66B0900}"/>
-    <hyperlink ref="A8" r:id="rId29" location="/56-color-silver_grey_anodized/40-length-500mm" xr:uid="{9A5B5164-04BD-4A3E-ACAD-59FF2E28D282}"/>
-    <hyperlink ref="A9" r:id="rId30" location="/56-color-silver_grey_anodized/40-length-500mm" xr:uid="{333EDDC9-F71F-4D00-9584-72AEF9E03D05}"/>
-    <hyperlink ref="B9" r:id="rId31" xr:uid="{3AAF8599-BF8E-4608-94BF-F3B9E7A7877D}"/>
-    <hyperlink ref="A27" r:id="rId32" xr:uid="{F4848447-A7E5-4981-8ED6-5ACCC059FBFD}"/>
-    <hyperlink ref="A42" r:id="rId33" xr:uid="{599CC434-2A6F-4512-9E0C-23C6EEDFFD8B}"/>
+    <hyperlink ref="A13" r:id="rId26" xr:uid="{9833C20E-591F-42B7-828C-80D603985010}"/>
+    <hyperlink ref="A10" r:id="rId27" xr:uid="{F713CD95-16C8-4DB2-AAAF-F46DD66B0900}"/>
+    <hyperlink ref="A8" r:id="rId28" location="/56-color-silver_grey_anodized/40-length-500mm" xr:uid="{9A5B5164-04BD-4A3E-ACAD-59FF2E28D282}"/>
+    <hyperlink ref="A9" r:id="rId29" location="/56-color-silver_grey_anodized/40-length-500mm" xr:uid="{333EDDC9-F71F-4D00-9584-72AEF9E03D05}"/>
+    <hyperlink ref="B9" r:id="rId30" xr:uid="{3AAF8599-BF8E-4608-94BF-F3B9E7A7877D}"/>
+    <hyperlink ref="A27" r:id="rId31" xr:uid="{F4848447-A7E5-4981-8ED6-5ACCC059FBFD}"/>
+    <hyperlink ref="A42" r:id="rId32" xr:uid="{599CC434-2A6F-4512-9E0C-23C6EEDFFD8B}"/>
+    <hyperlink ref="B7" r:id="rId33" xr:uid="{502D21A4-9549-4BDB-AA4F-4ED688D6848D}"/>
+    <hyperlink ref="A38" r:id="rId34" xr:uid="{33CF47E8-94F9-4FF4-8FC9-49C84931FE65}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
-  <drawing r:id="rId35"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
+  <drawing r:id="rId36"/>
 </worksheet>
 </file>
 
@@ -2272,30 +2272,30 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="29.25" x14ac:dyDescent="0.6">
+      <c r="B6" s="7" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.75">
-      <c r="B6" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>30</v>
       </c>
@@ -2303,21 +2303,21 @@
         <v>22</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="11">
         <v>25</v>
@@ -2330,12 +2330,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="12">
         <v>25</v>
@@ -2348,9 +2348,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>23</v>
@@ -2366,7 +2366,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>10</v>
       </c>
@@ -2402,12 +2402,12 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>40</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="C13" s="12">
         <v>10</v>
@@ -2420,12 +2420,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C14" s="12">
         <v>10</v>
@@ -2438,12 +2438,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="11">
         <v>10</v>
@@ -2456,7 +2456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>18</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
@@ -2492,12 +2492,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C18" s="12">
         <v>25</v>
@@ -2510,9 +2510,9 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>25</v>
@@ -2528,12 +2528,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="12">
         <v>40</v>
@@ -2546,7 +2546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
         <v>31</v>
       </c>
@@ -2564,7 +2564,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
         <v>4</v>
       </c>
@@ -2582,12 +2582,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="12">
         <v>150</v>
@@ -2600,7 +2600,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
         <v>7</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>26</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>27</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>19</v>
       </c>
@@ -2672,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
         <v>13</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
         <v>11</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
         <v>29</v>
       </c>
@@ -2726,12 +2726,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
         <v>24</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C31" s="12">
         <v>25</v>
@@ -2744,34 +2744,34 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E32" s="21">
         <f>SUM(E8:E31)</f>
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B34" s="14" t="s">
         <v>22</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:E31">
+  <sortState ref="A8:E31">
     <sortCondition ref="A8:A31"/>
   </sortState>
   <hyperlinks>

</xml_diff>